<commit_message>
added HM filter and mu_xwalk_summary table/chart
</commit_message>
<xml_diff>
--- a/MissingMapUnits2001_vs_crosswalk4.xlsx
+++ b/MissingMapUnits2001_vs_crosswalk4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\temp\mu_xwalks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Git_Repositories\mu_xwalk_2001_2011\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="0" windowWidth="18195" windowHeight="5730"/>
+    <workbookView xWindow="2925" yWindow="0" windowWidth="18195" windowHeight="5730" tabRatio="764" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MissingMapUnits2001_vs_crosswal" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="135">
   <si>
     <t>intLSGapMapCode</t>
   </si>
@@ -515,234 +515,6 @@
     <t>xwalk table</t>
   </si>
   <si>
-    <t>9912-4206
-South-Central Interior / Upper Coastal Plain Wet Flatwoods  TO  South-Central Interior / Upper Coastal Plain Wet Flatwoods</t>
-  </si>
-  <si>
-    <t>9912-4206</t>
-  </si>
-  <si>
-    <t>9912-4206
-South-Central Interior / Upper Coastal Plain Wet Flatwoods  TO
-  South-Central Interior / Upper Coastal Plain Wet Flatwoods</t>
-  </si>
-  <si>
-    <t>9855-9825
-Inter-Mountain Basins Montane Riparian Systems  TO  Rocky Mountain Lower Montane Riparian Woodland and Shrubland</t>
-  </si>
-  <si>
-    <t>9855-9825</t>
-  </si>
-  <si>
-    <t>9855-9825
-Inter-Mountain Basins Montane Riparian Systems  TO
-  Rocky Mountain Lower Montane Riparian Woodland and Shrubland</t>
-  </si>
-  <si>
-    <t>9601-9240
-Northern Atlantic Coastal Plain Pitch Pine Lowland  TO  Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</t>
-  </si>
-  <si>
-    <t>9601-9240</t>
-  </si>
-  <si>
-    <t>9601-9240
-Northern Atlantic Coastal Plain Pitch Pine Lowland  TO
-  Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</t>
-  </si>
-  <si>
-    <t>9402-9214
-Great Lakes Wooded Dune and Swale  TO  Laurentian-Acadian Swamp Systems</t>
-  </si>
-  <si>
-    <t>9402-9214</t>
-  </si>
-  <si>
-    <t>9402-9214
-Great Lakes Wooded Dune and Swale  TO
-  Laurentian-Acadian Swamp Systems</t>
-  </si>
-  <si>
-    <t>9308-9214
-Laurentian-Acadian Alkaline Conifer-Hardwood Swamp  TO  Laurentian-Acadian Swamp Systems</t>
-  </si>
-  <si>
-    <t>9308-9214</t>
-  </si>
-  <si>
-    <t>9308-9214
-Laurentian-Acadian Alkaline Conifer-Hardwood Swamp  TO
-  Laurentian-Acadian Swamp Systems</t>
-  </si>
-  <si>
-    <t>9242-9221
-Laurentian-Acadian Freshwater Marsh  TO  Great Lakes Coastal Marsh Systems</t>
-  </si>
-  <si>
-    <t>9242-9214</t>
-  </si>
-  <si>
-    <t>9242-9221
-Laurentian-Acadian Freshwater Marsh  TO
-  Great Lakes Coastal Marsh Systems</t>
-  </si>
-  <si>
-    <t>9234-9221
-Northern Great Lakes Coastal Marsh  TO  Great Lakes Coastal Marsh Systems</t>
-  </si>
-  <si>
-    <t>9234-9221</t>
-  </si>
-  <si>
-    <t>9234-9221
-Northern Great Lakes Coastal Marsh  TO
-  Great Lakes Coastal Marsh Systems</t>
-  </si>
-  <si>
-    <t>9229-9221
-Great Lakes Freshwater Estuary and Delta  TO  Great Lakes Coastal Marsh Systems</t>
-  </si>
-  <si>
-    <t>9229-9221</t>
-  </si>
-  <si>
-    <t>9229-9221
-Great Lakes Freshwater Estuary and Delta  TO
-  Great Lakes Coastal Marsh Systems</t>
-  </si>
-  <si>
-    <t>8503-8407
-Ruderal Upland - Old Field  TO  Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
-  </si>
-  <si>
-    <t>8503-8407</t>
-  </si>
-  <si>
-    <t>8503-8407
-Ruderal Upland - Old Field  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
-  </si>
-  <si>
-    <t>8405-8407
-Introduced Upland Vegetation - Perennial Grassland  TO  Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
-  </si>
-  <si>
-    <t>8405-8407</t>
-  </si>
-  <si>
-    <t>8405-8407
-Introduced Upland Vegetation - Perennial Grassland  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
-  </si>
-  <si>
-    <t>8403-8402
-Introduced Upland Vegetation - Forbland  TO  Introduced Upland Vegetation - Shrub</t>
-  </si>
-  <si>
-    <t>8403-8407</t>
-  </si>
-  <si>
-    <t>8403-8402
-Introduced Upland Vegetation - Forbland  TO
-  Introduced Upland Vegetation - Shrub</t>
-  </si>
-  <si>
-    <t>8105-8402
-Successional Shrub/Scrub (Other)  TO  Introduced Upland Vegetation - Shrub</t>
-  </si>
-  <si>
-    <t>8105-8402</t>
-  </si>
-  <si>
-    <t>8105-8402
-Successional Shrub/Scrub (Other)  TO
-  Introduced Upland Vegetation - Shrub</t>
-  </si>
-  <si>
-    <t>8104-8402
-Utility Swath - Herbaceous  TO  Introduced Upland Vegetation - Shrub</t>
-  </si>
-  <si>
-    <t>8104-8402</t>
-  </si>
-  <si>
-    <t>8104-8402
-Utility Swath - Herbaceous  TO
-  Introduced Upland Vegetation - Shrub</t>
-  </si>
-  <si>
-    <t>5108-5812
-Northern Rocky Mountain Avalanche Chute Shrubland  TO  Northern Rocky Mountain Subalpine Deciduous Shrubland</t>
-  </si>
-  <si>
-    <t>5108-5812</t>
-  </si>
-  <si>
-    <t>5108-5812
-Northern Rocky Mountain Avalanche Chute Shrubland  TO
-  Northern Rocky Mountain Subalpine Deciduous Shrubland</t>
-  </si>
-  <si>
-    <t>4542-5515
-Laurentian Jack Pine-Red Pine Forest  TO  Laurentian Pine-Oak Barrens</t>
-  </si>
-  <si>
-    <t>4542-5515</t>
-  </si>
-  <si>
-    <t>4542-5515
-Laurentian Jack Pine-Red Pine Forest  TO
-  Laurentian Pine-Oak Barrens</t>
-  </si>
-  <si>
-    <t>4142-9213
-East-Central Texas Plains Floodplain Forest  TO  Gulf and Atlantic Coastal Plain Swamp Systems</t>
-  </si>
-  <si>
-    <t>4142-9213</t>
-  </si>
-  <si>
-    <t>4142-9213
-East-Central Texas Plains Floodplain Forest  TO
-  Gulf and Atlantic Coastal Plain Swamp Systems</t>
-  </si>
-  <si>
-    <t>3204-3206
-Great Lakes Acidic Rocky Shore and Cliff  TO  Central Interior Acidic Cliff and Talus</t>
-  </si>
-  <si>
-    <t>3204-3206</t>
-  </si>
-  <si>
-    <t>3204-3206
-Great Lakes Acidic Rocky Shore and Cliff  TO
-  Central Interior Acidic Cliff and Talus</t>
-  </si>
-  <si>
-    <t>3109-3110
-Unconsolidated Shore (Beach/Dune)  TO  Unconsolidated Shore</t>
-  </si>
-  <si>
-    <t>3109-3110</t>
-  </si>
-  <si>
-    <t>3109-3110
-Unconsolidated Shore (Beach/Dune)  TO
-  Unconsolidated Shore</t>
-  </si>
-  <si>
-    <t>3108-3110
-Unconsolidated Shore (Lake/River/Pond)  TO  Unconsolidated Shore</t>
-  </si>
-  <si>
-    <t>3108-3110</t>
-  </si>
-  <si>
-    <t>3108-3110
-Unconsolidated Shore (Lake/River/Pond)  TO
-  Unconsolidated Shore</t>
-  </si>
-  <si>
     <t>1-1 (present-present)</t>
   </si>
   <si>
@@ -756,6 +528,69 @@
   </si>
   <si>
     <t>xwalk</t>
+  </si>
+  <si>
+    <t>mu_2001</t>
+  </si>
+  <si>
+    <t>mu_2011</t>
+  </si>
+  <si>
+    <t>3108-3110    Unconsolidated Shore (Lake/River/Pond) TO Unconsolidated Shore</t>
+  </si>
+  <si>
+    <t>3109-3110    Unconsolidated Shore (Beach/Dune) TO Unconsolidated Shore</t>
+  </si>
+  <si>
+    <t>3204-3206    Great Lakes Acidic Rocky Shore and Cliff TO Central Interior Acidic Cliff and Talus</t>
+  </si>
+  <si>
+    <t>4142-9213    East-Central Texas Plains Floodplain Forest TO Gulf and Atlantic Coastal Plain Swamp Systems</t>
+  </si>
+  <si>
+    <t>4542-5515    Laurentian Jack Pine-Red Pine Forest TO Laurentian Pine-Oak Barrens</t>
+  </si>
+  <si>
+    <t>5108-5812    Northern Rocky Mountain Avalanche Chute Shrubland TO Northern Rocky Mountain Subalpine Deciduous Shrubland</t>
+  </si>
+  <si>
+    <t>8104-8402    Utility Swath - Herbaceous TO Introduced Upland Vegetation - Shrub</t>
+  </si>
+  <si>
+    <t>8105-8402    Successional Shrub/Scrub (Other) TO Introduced Upland Vegetation - Shrub</t>
+  </si>
+  <si>
+    <t>8403-8407    Introduced Upland Vegetation - Forbland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
+  </si>
+  <si>
+    <t>8405-8407    Introduced Upland Vegetation - Perennial Grassland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
+  </si>
+  <si>
+    <t>8503-8407    Ruderal Upland - Old Field TO Introduced Upland Vegetation - Perennial Grassland and Forbland</t>
+  </si>
+  <si>
+    <t>9229-9221    Great Lakes Freshwater Estuary and Delta TO Great Lakes Coastal Marsh Systems</t>
+  </si>
+  <si>
+    <t>9234-9221    Northern Great Lakes Coastal Marsh TO Great Lakes Coastal Marsh Systems</t>
+  </si>
+  <si>
+    <t>9242-9214    Laurentian-Acadian Freshwater Marsh TO Laurentian-Acadian Swamp Systems</t>
+  </si>
+  <si>
+    <t>9308-9214    Laurentian-Acadian Alkaline Conifer-Hardwood Swamp TO Laurentian-Acadian Swamp Systems</t>
+  </si>
+  <si>
+    <t>9402-9214    Great Lakes Wooded Dune and Swale TO Laurentian-Acadian Swamp Systems</t>
+  </si>
+  <si>
+    <t>9601-9240    Northern Atlantic Coastal Plain Pitch Pine Lowland TO Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</t>
+  </si>
+  <si>
+    <t>9855-9825    Inter-Mountain Basins Montane Riparian Systems TO Rocky Mountain Lower Montane Riparian Woodland and Shrubland</t>
+  </si>
+  <si>
+    <t>9912-4206    South-Central Interior / Upper Coastal Plain Wet Flatwoods TO South-Central Interior / Upper Coastal Plain Flatwoods</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1206,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1516,9 +1351,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1691,7 +1523,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$C$1</c:f>
+              <c:f>mu_xwalk_summary!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1716,110 +1548,72 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$A$2:$A$20</c:f>
+              <c:f>mu_xwalk_summary!$C$2:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3108-3110
-Unconsolidated Shore (Lake/River/Pond)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3108-3110    Unconsolidated Shore (Lake/River/Pond) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3109-3110
-Unconsolidated Shore (Beach/Dune)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3109-3110    Unconsolidated Shore (Beach/Dune) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3204-3206
-Great Lakes Acidic Rocky Shore and Cliff  TO
-  Central Interior Acidic Cliff and Talus</c:v>
+                  <c:v>3204-3206    Great Lakes Acidic Rocky Shore and Cliff TO Central Interior Acidic Cliff and Talus</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4142-9213
-East-Central Texas Plains Floodplain Forest  TO
-  Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
+                  <c:v>4142-9213    East-Central Texas Plains Floodplain Forest TO Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4542-5515
-Laurentian Jack Pine-Red Pine Forest  TO
-  Laurentian Pine-Oak Barrens</c:v>
+                  <c:v>4542-5515    Laurentian Jack Pine-Red Pine Forest TO Laurentian Pine-Oak Barrens</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5108-5812
-Northern Rocky Mountain Avalanche Chute Shrubland  TO
-  Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
+                  <c:v>5108-5812    Northern Rocky Mountain Avalanche Chute Shrubland TO Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8104-8402
-Utility Swath - Herbaceous  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8104-8402    Utility Swath - Herbaceous TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8105-8402
-Successional Shrub/Scrub (Other)  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8105-8402    Successional Shrub/Scrub (Other) TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8403-8402
-Introduced Upland Vegetation - Forbland  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8403-8407    Introduced Upland Vegetation - Forbland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8405-8407
-Introduced Upland Vegetation - Perennial Grassland  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8405-8407    Introduced Upland Vegetation - Perennial Grassland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8503-8407
-Ruderal Upland - Old Field  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8503-8407    Ruderal Upland - Old Field TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9229-9221
-Great Lakes Freshwater Estuary and Delta  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9229-9221    Great Lakes Freshwater Estuary and Delta TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9234-9221
-Northern Great Lakes Coastal Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9234-9221    Northern Great Lakes Coastal Marsh TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9242-9221
-Laurentian-Acadian Freshwater Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9242-9214    Laurentian-Acadian Freshwater Marsh TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9308-9214
-Laurentian-Acadian Alkaline Conifer-Hardwood Swamp  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9308-9214    Laurentian-Acadian Alkaline Conifer-Hardwood Swamp TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9402-9214
-Great Lakes Wooded Dune and Swale  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9402-9214    Great Lakes Wooded Dune and Swale TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9601-9240
-Northern Atlantic Coastal Plain Pitch Pine Lowland  TO
-  Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
+                  <c:v>9601-9240    Northern Atlantic Coastal Plain Pitch Pine Lowland TO Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9855-9825
-Inter-Mountain Basins Montane Riparian Systems  TO
-  Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
+                  <c:v>9855-9825    Inter-Mountain Basins Montane Riparian Systems TO Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9912-4206
-South-Central Interior / Upper Coastal Plain Wet Flatwoods  TO
-  South-Central Interior / Upper Coastal Plain Wet Flatwoods</c:v>
+                  <c:v>9912-4206    South-Central Interior / Upper Coastal Plain Wet Flatwoods TO South-Central Interior / Upper Coastal Plain Flatwoods</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mu_xwalk_summary!$C$2:$C$20</c:f>
+              <c:f>mu_xwalk_summary!$D$2:$D$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1889,7 +1683,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$D$1</c:f>
+              <c:f>mu_xwalk_summary!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1911,110 +1705,72 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$A$2:$A$20</c:f>
+              <c:f>mu_xwalk_summary!$C$2:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3108-3110
-Unconsolidated Shore (Lake/River/Pond)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3108-3110    Unconsolidated Shore (Lake/River/Pond) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3109-3110
-Unconsolidated Shore (Beach/Dune)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3109-3110    Unconsolidated Shore (Beach/Dune) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3204-3206
-Great Lakes Acidic Rocky Shore and Cliff  TO
-  Central Interior Acidic Cliff and Talus</c:v>
+                  <c:v>3204-3206    Great Lakes Acidic Rocky Shore and Cliff TO Central Interior Acidic Cliff and Talus</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4142-9213
-East-Central Texas Plains Floodplain Forest  TO
-  Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
+                  <c:v>4142-9213    East-Central Texas Plains Floodplain Forest TO Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4542-5515
-Laurentian Jack Pine-Red Pine Forest  TO
-  Laurentian Pine-Oak Barrens</c:v>
+                  <c:v>4542-5515    Laurentian Jack Pine-Red Pine Forest TO Laurentian Pine-Oak Barrens</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5108-5812
-Northern Rocky Mountain Avalanche Chute Shrubland  TO
-  Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
+                  <c:v>5108-5812    Northern Rocky Mountain Avalanche Chute Shrubland TO Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8104-8402
-Utility Swath - Herbaceous  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8104-8402    Utility Swath - Herbaceous TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8105-8402
-Successional Shrub/Scrub (Other)  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8105-8402    Successional Shrub/Scrub (Other) TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8403-8402
-Introduced Upland Vegetation - Forbland  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8403-8407    Introduced Upland Vegetation - Forbland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8405-8407
-Introduced Upland Vegetation - Perennial Grassland  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8405-8407    Introduced Upland Vegetation - Perennial Grassland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8503-8407
-Ruderal Upland - Old Field  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8503-8407    Ruderal Upland - Old Field TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9229-9221
-Great Lakes Freshwater Estuary and Delta  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9229-9221    Great Lakes Freshwater Estuary and Delta TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9234-9221
-Northern Great Lakes Coastal Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9234-9221    Northern Great Lakes Coastal Marsh TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9242-9221
-Laurentian-Acadian Freshwater Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9242-9214    Laurentian-Acadian Freshwater Marsh TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9308-9214
-Laurentian-Acadian Alkaline Conifer-Hardwood Swamp  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9308-9214    Laurentian-Acadian Alkaline Conifer-Hardwood Swamp TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9402-9214
-Great Lakes Wooded Dune and Swale  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9402-9214    Great Lakes Wooded Dune and Swale TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9601-9240
-Northern Atlantic Coastal Plain Pitch Pine Lowland  TO
-  Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
+                  <c:v>9601-9240    Northern Atlantic Coastal Plain Pitch Pine Lowland TO Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9855-9825
-Inter-Mountain Basins Montane Riparian Systems  TO
-  Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
+                  <c:v>9855-9825    Inter-Mountain Basins Montane Riparian Systems TO Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9912-4206
-South-Central Interior / Upper Coastal Plain Wet Flatwoods  TO
-  South-Central Interior / Upper Coastal Plain Wet Flatwoods</c:v>
+                  <c:v>9912-4206    South-Central Interior / Upper Coastal Plain Wet Flatwoods TO South-Central Interior / Upper Coastal Plain Flatwoods</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mu_xwalk_summary!$D$2:$D$20</c:f>
+              <c:f>mu_xwalk_summary!$E$2:$E$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2084,7 +1840,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$E$1</c:f>
+              <c:f>mu_xwalk_summary!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2106,110 +1862,72 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$A$2:$A$20</c:f>
+              <c:f>mu_xwalk_summary!$C$2:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3108-3110
-Unconsolidated Shore (Lake/River/Pond)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3108-3110    Unconsolidated Shore (Lake/River/Pond) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3109-3110
-Unconsolidated Shore (Beach/Dune)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3109-3110    Unconsolidated Shore (Beach/Dune) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3204-3206
-Great Lakes Acidic Rocky Shore and Cliff  TO
-  Central Interior Acidic Cliff and Talus</c:v>
+                  <c:v>3204-3206    Great Lakes Acidic Rocky Shore and Cliff TO Central Interior Acidic Cliff and Talus</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4142-9213
-East-Central Texas Plains Floodplain Forest  TO
-  Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
+                  <c:v>4142-9213    East-Central Texas Plains Floodplain Forest TO Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4542-5515
-Laurentian Jack Pine-Red Pine Forest  TO
-  Laurentian Pine-Oak Barrens</c:v>
+                  <c:v>4542-5515    Laurentian Jack Pine-Red Pine Forest TO Laurentian Pine-Oak Barrens</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5108-5812
-Northern Rocky Mountain Avalanche Chute Shrubland  TO
-  Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
+                  <c:v>5108-5812    Northern Rocky Mountain Avalanche Chute Shrubland TO Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8104-8402
-Utility Swath - Herbaceous  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8104-8402    Utility Swath - Herbaceous TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8105-8402
-Successional Shrub/Scrub (Other)  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8105-8402    Successional Shrub/Scrub (Other) TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8403-8402
-Introduced Upland Vegetation - Forbland  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8403-8407    Introduced Upland Vegetation - Forbland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8405-8407
-Introduced Upland Vegetation - Perennial Grassland  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8405-8407    Introduced Upland Vegetation - Perennial Grassland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8503-8407
-Ruderal Upland - Old Field  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8503-8407    Ruderal Upland - Old Field TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9229-9221
-Great Lakes Freshwater Estuary and Delta  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9229-9221    Great Lakes Freshwater Estuary and Delta TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9234-9221
-Northern Great Lakes Coastal Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9234-9221    Northern Great Lakes Coastal Marsh TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9242-9221
-Laurentian-Acadian Freshwater Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9242-9214    Laurentian-Acadian Freshwater Marsh TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9308-9214
-Laurentian-Acadian Alkaline Conifer-Hardwood Swamp  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9308-9214    Laurentian-Acadian Alkaline Conifer-Hardwood Swamp TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9402-9214
-Great Lakes Wooded Dune and Swale  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9402-9214    Great Lakes Wooded Dune and Swale TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9601-9240
-Northern Atlantic Coastal Plain Pitch Pine Lowland  TO
-  Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
+                  <c:v>9601-9240    Northern Atlantic Coastal Plain Pitch Pine Lowland TO Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9855-9825
-Inter-Mountain Basins Montane Riparian Systems  TO
-  Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
+                  <c:v>9855-9825    Inter-Mountain Basins Montane Riparian Systems TO Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9912-4206
-South-Central Interior / Upper Coastal Plain Wet Flatwoods  TO
-  South-Central Interior / Upper Coastal Plain Wet Flatwoods</c:v>
+                  <c:v>9912-4206    South-Central Interior / Upper Coastal Plain Wet Flatwoods TO South-Central Interior / Upper Coastal Plain Flatwoods</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mu_xwalk_summary!$E$2:$E$20</c:f>
+              <c:f>mu_xwalk_summary!$F$2:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2279,7 +1997,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$F$1</c:f>
+              <c:f>mu_xwalk_summary!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2303,110 +2021,72 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>mu_xwalk_summary!$A$2:$A$20</c:f>
+              <c:f>mu_xwalk_summary!$C$2:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3108-3110
-Unconsolidated Shore (Lake/River/Pond)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3108-3110    Unconsolidated Shore (Lake/River/Pond) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3109-3110
-Unconsolidated Shore (Beach/Dune)  TO
-  Unconsolidated Shore</c:v>
+                  <c:v>3109-3110    Unconsolidated Shore (Beach/Dune) TO Unconsolidated Shore</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3204-3206
-Great Lakes Acidic Rocky Shore and Cliff  TO
-  Central Interior Acidic Cliff and Talus</c:v>
+                  <c:v>3204-3206    Great Lakes Acidic Rocky Shore and Cliff TO Central Interior Acidic Cliff and Talus</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4142-9213
-East-Central Texas Plains Floodplain Forest  TO
-  Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
+                  <c:v>4142-9213    East-Central Texas Plains Floodplain Forest TO Gulf and Atlantic Coastal Plain Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4542-5515
-Laurentian Jack Pine-Red Pine Forest  TO
-  Laurentian Pine-Oak Barrens</c:v>
+                  <c:v>4542-5515    Laurentian Jack Pine-Red Pine Forest TO Laurentian Pine-Oak Barrens</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5108-5812
-Northern Rocky Mountain Avalanche Chute Shrubland  TO
-  Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
+                  <c:v>5108-5812    Northern Rocky Mountain Avalanche Chute Shrubland TO Northern Rocky Mountain Subalpine Deciduous Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8104-8402
-Utility Swath - Herbaceous  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8104-8402    Utility Swath - Herbaceous TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8105-8402
-Successional Shrub/Scrub (Other)  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8105-8402    Successional Shrub/Scrub (Other) TO Introduced Upland Vegetation - Shrub</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8403-8402
-Introduced Upland Vegetation - Forbland  TO
-  Introduced Upland Vegetation - Shrub</c:v>
+                  <c:v>8403-8407    Introduced Upland Vegetation - Forbland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8405-8407
-Introduced Upland Vegetation - Perennial Grassland  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8405-8407    Introduced Upland Vegetation - Perennial Grassland TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8503-8407
-Ruderal Upland - Old Field  TO
-  Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
+                  <c:v>8503-8407    Ruderal Upland - Old Field TO Introduced Upland Vegetation - Perennial Grassland and Forbland</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9229-9221
-Great Lakes Freshwater Estuary and Delta  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9229-9221    Great Lakes Freshwater Estuary and Delta TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9234-9221
-Northern Great Lakes Coastal Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9234-9221    Northern Great Lakes Coastal Marsh TO Great Lakes Coastal Marsh Systems</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9242-9221
-Laurentian-Acadian Freshwater Marsh  TO
-  Great Lakes Coastal Marsh Systems</c:v>
+                  <c:v>9242-9214    Laurentian-Acadian Freshwater Marsh TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9308-9214
-Laurentian-Acadian Alkaline Conifer-Hardwood Swamp  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9308-9214    Laurentian-Acadian Alkaline Conifer-Hardwood Swamp TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9402-9214
-Great Lakes Wooded Dune and Swale  TO
-  Laurentian-Acadian Swamp Systems</c:v>
+                  <c:v>9402-9214    Great Lakes Wooded Dune and Swale TO Laurentian-Acadian Swamp Systems</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9601-9240
-Northern Atlantic Coastal Plain Pitch Pine Lowland  TO
-  Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
+                  <c:v>9601-9240    Northern Atlantic Coastal Plain Pitch Pine Lowland TO Northern Atlantic Coastal Plain Basin Swamp and Wet Hardwood Forest</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9855-9825
-Inter-Mountain Basins Montane Riparian Systems  TO
-  Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
+                  <c:v>9855-9825    Inter-Mountain Basins Montane Riparian Systems TO Rocky Mountain Lower Montane Riparian Woodland and Shrubland</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9912-4206
-South-Central Interior / Upper Coastal Plain Wet Flatwoods  TO
-  South-Central Interior / Upper Coastal Plain Wet Flatwoods</c:v>
+                  <c:v>9912-4206    South-Central Interior / Upper Coastal Plain Wet Flatwoods TO South-Central Interior / Upper Coastal Plain Flatwoods</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mu_xwalk_summary!$F$2:$F$20</c:f>
+              <c:f>mu_xwalk_summary!$G$2:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -2481,12 +2161,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="549746048"/>
-        <c:axId val="549747168"/>
+        <c:axId val="232206880"/>
+        <c:axId val="232208560"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="549746048"/>
+        <c:axId val="232206880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2523,7 +2203,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549747168"/>
+        <c:crossAx val="232208560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2531,7 +2211,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="549747168"/>
+        <c:axId val="232208560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2582,7 +2262,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549746048"/>
+        <c:crossAx val="232206880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3533,7 +3213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O3" sqref="O3:O21"/>
     </sheetView>
@@ -4769,582 +4449,475 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.28515625" customWidth="1"/>
-    <col min="10" max="10" width="91.28515625" customWidth="1"/>
+    <col min="3" max="3" width="91.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
       <c r="B1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3108</v>
+      </c>
+      <c r="B2">
+        <v>3110</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2">
         <v>4417</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>189</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>66</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>843</v>
       </c>
-      <c r="H2" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3109</v>
+      </c>
+      <c r="B3">
+        <v>3110</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3">
         <v>4441</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>225</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>42</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>807</v>
       </c>
-      <c r="H3" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3204</v>
+      </c>
+      <c r="B4">
+        <v>3206</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4">
         <v>5294</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>103</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>30</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>88</v>
       </c>
-      <c r="H4" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="51" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4142</v>
+      </c>
+      <c r="B5">
+        <v>9213</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>4857</v>
+      </c>
+      <c r="E5">
+        <v>226</v>
+      </c>
+      <c r="F5">
+        <v>332</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4542</v>
+      </c>
+      <c r="B6">
+        <v>5515</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>5162</v>
+      </c>
+      <c r="E6">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
+      </c>
+      <c r="G6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5108</v>
+      </c>
+      <c r="B7">
+        <v>5812</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7">
+        <v>5083</v>
+      </c>
+      <c r="E7">
+        <v>261</v>
+      </c>
+      <c r="F7">
+        <v>48</v>
+      </c>
+      <c r="G7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8104</v>
+      </c>
+      <c r="B8">
+        <v>8402</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8">
+        <v>3834</v>
+      </c>
+      <c r="E8">
+        <v>394</v>
+      </c>
+      <c r="F8">
+        <v>716</v>
+      </c>
+      <c r="G8">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8105</v>
+      </c>
+      <c r="B9">
+        <v>8402</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9">
+        <v>4345</v>
+      </c>
+      <c r="E9">
+        <v>188</v>
+      </c>
+      <c r="F9">
+        <v>205</v>
+      </c>
+      <c r="G9">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8403</v>
+      </c>
+      <c r="B10">
+        <v>8407</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10">
+        <v>3837</v>
+      </c>
+      <c r="E10">
+        <v>323</v>
+      </c>
+      <c r="F10">
+        <v>113</v>
+      </c>
+      <c r="G10">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8405</v>
+      </c>
+      <c r="B11">
+        <v>8407</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11">
+        <v>3803</v>
+      </c>
+      <c r="E11">
+        <v>302</v>
+      </c>
+      <c r="F11">
+        <v>147</v>
+      </c>
+      <c r="G11">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8503</v>
+      </c>
+      <c r="B12">
+        <v>8407</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12">
+        <v>3693</v>
+      </c>
+      <c r="E12">
+        <v>431</v>
+      </c>
+      <c r="F12">
+        <v>257</v>
+      </c>
+      <c r="G12">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9229</v>
+      </c>
+      <c r="B13">
+        <v>9221</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <v>5054</v>
+      </c>
+      <c r="E13">
+        <v>49</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9234</v>
+      </c>
+      <c r="B14">
+        <v>9221</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14">
+        <v>5044</v>
+      </c>
+      <c r="E14">
+        <v>127</v>
+      </c>
+      <c r="F14">
+        <v>21</v>
+      </c>
+      <c r="G14">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9242</v>
+      </c>
+      <c r="B15">
+        <v>9214</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15">
+        <v>4933</v>
+      </c>
+      <c r="E15">
+        <v>244</v>
+      </c>
+      <c r="F15">
+        <v>198</v>
+      </c>
+      <c r="G15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9308</v>
+      </c>
+      <c r="B16">
+        <v>9214</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16">
+        <v>4952</v>
+      </c>
+      <c r="E16">
+        <v>33</v>
+      </c>
+      <c r="F16">
+        <v>179</v>
+      </c>
+      <c r="G16">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9402</v>
+      </c>
+      <c r="B17">
+        <v>9214</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17">
+        <v>4985</v>
+      </c>
+      <c r="E17">
+        <v>244</v>
+      </c>
+      <c r="F17">
+        <v>146</v>
+      </c>
+      <c r="G17">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>9601</v>
+      </c>
+      <c r="B18">
+        <v>9240</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18">
+        <v>4850</v>
+      </c>
+      <c r="E18">
+        <v>440</v>
+      </c>
+      <c r="F18">
+        <v>26</v>
+      </c>
+      <c r="G18">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9855</v>
+      </c>
+      <c r="B19">
+        <v>9825</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19">
+        <v>4002</v>
+      </c>
+      <c r="E19">
+        <v>1081</v>
+      </c>
+      <c r="F19">
         <v>80</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5">
-        <v>4857</v>
-      </c>
-      <c r="D5">
-        <v>226</v>
-      </c>
-      <c r="E5">
-        <v>332</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="H5" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6">
-        <v>5162</v>
-      </c>
-      <c r="D6">
-        <v>118</v>
-      </c>
-      <c r="E6">
-        <v>101</v>
-      </c>
-      <c r="F6">
+      <c r="G19">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9912</v>
+      </c>
+      <c r="B20">
+        <v>4206</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H6" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7">
-        <v>5083</v>
-      </c>
-      <c r="D7">
-        <v>261</v>
-      </c>
-      <c r="E7">
-        <v>48</v>
-      </c>
-      <c r="F7">
-        <v>123</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8">
-        <v>3834</v>
-      </c>
-      <c r="D8">
-        <v>394</v>
-      </c>
-      <c r="E8">
-        <v>716</v>
-      </c>
-      <c r="F8">
-        <v>571</v>
-      </c>
-      <c r="H8" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9">
-        <v>4345</v>
-      </c>
-      <c r="D9">
-        <v>188</v>
-      </c>
-      <c r="E9">
-        <v>205</v>
-      </c>
-      <c r="F9">
-        <v>777</v>
-      </c>
-      <c r="H9" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10">
-        <v>3837</v>
-      </c>
-      <c r="D10">
-        <v>323</v>
-      </c>
-      <c r="E10">
-        <v>113</v>
-      </c>
-      <c r="F10">
-        <v>1242</v>
-      </c>
-      <c r="H10" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11">
-        <v>3803</v>
-      </c>
-      <c r="D11">
-        <v>302</v>
-      </c>
-      <c r="E11">
-        <v>147</v>
-      </c>
-      <c r="F11">
-        <v>1263</v>
-      </c>
-      <c r="H11" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12">
-        <v>3693</v>
-      </c>
-      <c r="D12">
-        <v>431</v>
-      </c>
-      <c r="E12">
-        <v>257</v>
-      </c>
-      <c r="F12">
-        <v>1134</v>
-      </c>
-      <c r="H12" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="51" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13">
-        <v>5054</v>
-      </c>
-      <c r="D13">
-        <v>49</v>
-      </c>
-      <c r="E13">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>401</v>
-      </c>
-      <c r="H13" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14">
-        <v>5044</v>
-      </c>
-      <c r="D14">
-        <v>127</v>
-      </c>
-      <c r="E14">
-        <v>21</v>
-      </c>
-      <c r="F14">
-        <v>323</v>
-      </c>
-      <c r="H14" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15">
-        <v>4933</v>
-      </c>
-      <c r="D15">
-        <v>244</v>
-      </c>
-      <c r="E15">
-        <v>198</v>
-      </c>
-      <c r="F15">
-        <v>140</v>
-      </c>
-      <c r="H15" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C16">
-        <v>4952</v>
-      </c>
-      <c r="D16">
-        <v>33</v>
-      </c>
-      <c r="E16">
-        <v>179</v>
-      </c>
-      <c r="F16">
-        <v>351</v>
-      </c>
-      <c r="H16" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17">
-        <v>4985</v>
-      </c>
-      <c r="D17">
-        <v>244</v>
-      </c>
-      <c r="E17">
-        <v>146</v>
-      </c>
-      <c r="F17">
-        <v>140</v>
-      </c>
-      <c r="H17" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C18">
-        <v>4850</v>
-      </c>
-      <c r="D18">
-        <v>440</v>
-      </c>
-      <c r="E18">
-        <v>26</v>
-      </c>
-      <c r="F18">
-        <v>199</v>
-      </c>
-      <c r="H18" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19">
-        <v>4002</v>
-      </c>
-      <c r="D19">
-        <v>1081</v>
-      </c>
-      <c r="E19">
-        <v>80</v>
-      </c>
-      <c r="F19">
-        <v>352</v>
-      </c>
-      <c r="H19" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20">
+      <c r="D20">
         <v>4841</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>12</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>189</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>473</v>
-      </c>
-      <c r="H20" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5356,7 +4929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>